<commit_message>
Update plan de test PCB mallette (1).xlsx
</commit_message>
<xml_diff>
--- a/Matériel/plan de test PCB mallette (1).xlsx
+++ b/Matériel/plan de test PCB mallette (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Matériel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142CECF6-CC1E-45A7-8170-5754FFB7C7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1884D9C-F4A2-4919-B67F-FEC8F41FDDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Fonction</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Tester pour les court-circuits avec un multimètre en mode résistance sur les pattes 5v et mise à terre</t>
   </si>
   <si>
-    <t>Tester la résistance entre les pattes des composants énergivores avec un multimètre en mode résistance sur les pattes 5v et la patte des pattes des Vin des composantes.</t>
-  </si>
-  <si>
     <t>Tester l'ergonomique de la poignée. Verifier s'il y a des angles coupants</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>il y a un short-circuit entre le VUSB et le GND. On va driller un trou dans les PCB pour régler ce problème</t>
   </si>
   <si>
-    <t>la longueur prévue pour le fils USB-C est un peu court. Nous allons devoir faire un petit loop</t>
-  </si>
-  <si>
     <t>Il n'y en a pas, ce n'est pas parce que l'on en a pas mis, mais sa semble être une erreur de fabrication, à cause que sur Altium la poigné est présente</t>
   </si>
   <si>
@@ -209,7 +203,19 @@
     <t xml:space="preserve">La pattes gpio10 du devrait être au gpio 19 ou 13. Pattes des strip de DEL. DONC LE RESET DE POT' ET LE BTN DEL DOIVENT ÊTRE CHANGÉ DE PLACE </t>
   </si>
   <si>
-    <t>Le pi n'a pas assez de courant pour alimenter tous et l'écran</t>
+    <t>Tester la résistance entre les pattes des composants énergivores avec un multimètre en mode résistance sur les pattes 5v et la patte des pattes des Vin des composantes pour éviter les court-circuit.</t>
+  </si>
+  <si>
+    <t>la longueur prévue pour le fils USB-C est un peu court. Nous allons devoir faire une boucle</t>
+  </si>
+  <si>
+    <t>Il faut reset les esp32 pour activer le i2c des esp32</t>
+  </si>
+  <si>
+    <t>L'écran demande trop de courant si on l'alimente du PI</t>
+  </si>
+  <si>
+    <t>Le pi n'a pas assez de courant pour alimenter tous et l'écran avec les ports USB-C du pi</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -643,6 +649,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A179C3DD-CE59-450A-90EC-B70C1216426A}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1309,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1318,152 +1327,170 @@
         <v>20</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E11" s="22"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:7" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" s="15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="22"/>
+      <c r="D18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="44"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="D21" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:6" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1501,7 +1528,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" s="37"/>
       <c r="E29" s="25"/>
@@ -1512,7 +1539,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -1523,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -1534,7 +1561,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -1545,7 +1572,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
@@ -1556,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -1636,6 +1663,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100579959CCCCA5C544BBD30F9226CE8516" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5ff6d6050dbb5268810d83a948b12d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88fb2577-ad7a-4d43-8167-cef18aea1aa3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85ed7a65d7fcb03429aa0547ee3ef026" ns2:_="">
     <xsd:import namespace="88fb2577-ad7a-4d43-8167-cef18aea1aa3"/>
@@ -1779,16 +1815,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E286483B-C6D9-4B9F-A304-E190CE0F1062}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91CA2F8A-2602-4339-82CB-7CAA9667905F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1804,12 +1839,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E286483B-C6D9-4B9F-A304-E190CE0F1062}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout reset esp32 et heartbeat
</commit_message>
<xml_diff>
--- a/Matériel/plan de test PCB mallette (1).xlsx
+++ b/Matériel/plan de test PCB mallette (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Matériel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07427248-BB4E-4676-8D35-E967B6C0A3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E1026-EC21-4B54-ABC4-4ECD1DDFAE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Fonction</t>
   </si>
@@ -170,24 +170,9 @@
     <t>Avec le programme python "integrationTotal" vérifier que tout les esp32 et leurs objets interactifs transmettent leurs donnèes et les affichent sur le mini écran.</t>
   </si>
   <si>
-    <t>il y a un short-circuit entre le VUSB et le GND. On va driller un trou dans les PCB pour régler ce problème</t>
-  </si>
-  <si>
-    <t>le pcb entre sans problème dans le fond de la mallette</t>
-  </si>
-  <si>
-    <t>les trous de montages du  Raspberry Pi sur le PCB sont parfaitement alignés</t>
-  </si>
-  <si>
-    <t>les trous de montage au travers de la mallette ne passent pas au travers des support en dessous de la mallette</t>
-  </si>
-  <si>
     <t>Ajouter une dead zone autour des points de montage du port USB-C, car il cause un court-circuit sinon</t>
   </si>
   <si>
-    <t>Les pattes du esp32 POT sont aux mauvaise endroit. Les patte gpio 9, gpio 8 et gpio 5 devrait être au gpio0, gpio1 et gpio2</t>
-  </si>
-  <si>
     <t>Les patte gpio 9, gpio 8 et gpio 5 du esp32 POT devrait être au gpio0, gpio1 et gpio2</t>
   </si>
   <si>
@@ -200,22 +185,28 @@
     <t>Tester la résistance entre les pattes des composants énergivores avec un multimètre en mode résistance sur les pattes 5v et la patte des pattes des Vin des composantes pour éviter les court-circuit.</t>
   </si>
   <si>
-    <t>la longueur prévue pour le fils USB-C est un peu court. Nous allons devoir faire une boucle</t>
-  </si>
-  <si>
-    <t>Il faut reset les esp32 pour activer le i2c des esp32</t>
-  </si>
-  <si>
-    <t>L'écran demande trop de courant si on l'alimente du PI</t>
-  </si>
-  <si>
     <t>Le pi n'a pas assez de courant pour alimenter tous et l'écran avec les ports USB-C du pi</t>
   </si>
   <si>
     <t xml:space="preserve">La pattes gpio10 du PI devrait être au gpio 19 ou 13. Pattes des strip de DEL. DONC LE RESET DE POT' ET LE BTN DEL DOIVENT ÊTRE CHANGÉ DE PLACE </t>
   </si>
   <si>
-    <t>Le frabricant n'a pas mis de poignée comme désigné sur le PCB. La poignée est bien là sur Altium. Une plainte a été lancé.</t>
+    <t>Le fabricant n'a pas mis de poignée comme désigné sur le PCB. La poignée est bien là sur Altium. Une plainte a été lancé.</t>
+  </si>
+  <si>
+    <t>il y a un short-circuit entre le VUSB et le GND au niveau des via de support du connecteur usb-c. Problèeme réglé en perçant un trou dans le via dans les PCB.</t>
+  </si>
+  <si>
+    <t>Il faut que les esp32 boot après le PI pour activer le i2c des esp32</t>
+  </si>
+  <si>
+    <t>L'écran demande trop de courant si on l'alimente à l'aide du PI</t>
+  </si>
+  <si>
+    <t>Les pots sont non fonctionnel. La DEL adressable au pin 10 est non fonctionnel. L'écran demande trop de courant si on l'alimente à l'aide du PI</t>
+  </si>
+  <si>
+    <t>Les resistance des SW ne sont pas dans le bon ordre, ils sont dans l'ordre 2,1,4,3,6,5,8,7 au lieu de 1,2,3,4,5,6,7,8</t>
   </si>
 </sst>
 </file>
@@ -1201,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A179C3DD-CE59-450A-90EC-B70C1216426A}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1318,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1327,7 +1318,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>9</v>
@@ -1346,7 +1337,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1360,9 +1351,7 @@
       <c r="D13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>47</v>
-      </c>
+      <c r="E13" s="22"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1375,9 +1364,7 @@
       <c r="D14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="E14" s="15"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1390,9 +1377,7 @@
       <c r="D15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>45</v>
-      </c>
+      <c r="E15" s="22"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1405,9 +1390,7 @@
       <c r="D16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -1475,7 +1458,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1490,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1528,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D29" s="37"/>
       <c r="E29" s="25"/>
@@ -1539,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -1550,7 +1533,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -1561,7 +1544,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -1572,7 +1555,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
@@ -1583,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -1593,7 +1576,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C35" s="25"/>
+      <c r="C35" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
     </row>

</xml_diff>

<commit_message>
update du plan de test
un bug à été découvert en rapport avec les dels
</commit_message>
<xml_diff>
--- a/Matériel/plan de test PCB mallette (1).xlsx
+++ b/Matériel/plan de test PCB mallette (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Matériel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\cours\planif projet\Projet_Final_TSO\Matériel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E1026-EC21-4B54-ABC4-4ECD1DDFAE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375D72DE-435A-4716-B1AA-238118741BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Fonction</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Les resistance des SW ne sont pas dans le bon ordre, ils sont dans l'ordre 2,1,4,3,6,5,8,7 au lieu de 1,2,3,4,5,6,7,8</t>
+  </si>
+  <si>
+    <t>Les GPIO 12 et 18 tout comme 13 et 19, partage le même PWM, ce qui provoque que les strip de dels vont avoir exactement le même signal. Il est donc uniquement possible d'avoir 3 strip de dels différentes en même temps</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A179C3DD-CE59-450A-90EC-B70C1216426A}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1587,7 +1590,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C36" s="25"/>
+      <c r="C36" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
     </row>

</xml_diff>